<commit_message>
hem4 runs from multi window and produces outputs on separate thread but loses callbacks so no logs
</commit_message>
<xml_diff>
--- a/fixtures/input/hapemis.xlsx
+++ b/fixtures/input/hapemis.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jbaker\Documents\HEM4Python\Version1.0\sample files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David Lindsey\OneDrive - SC&amp;A, Inc\HEM4Python\Version_Master\fixtures\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_ED6EE65C31EAAB3EB31984B3486DB4A50362AFBE" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{5742F092-93D8-4F3F-B260-63D537A938D7}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19170" windowHeight="7665" xr2:uid="{84215347-E9F3-436D-9697-2FCBE894B50C}"/>
   </bookViews>
@@ -421,6 +422,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="22.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">

</xml_diff>